<commit_message>
correct whitespace in colour names
</commit_message>
<xml_diff>
--- a/aux/master-spreadsheet.xlsx
+++ b/aux/master-spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\09_next_projects\SEC\SEC-card-game\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84EE2136-1A36-4B76-AC3B-2FF85D69F5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A5D2D9-3246-435D-977D-E797F7AB3F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{F8231788-E26F-497A-84D5-4BB029B3585E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8231788-E26F-497A-84D5-4BB029B3585E}"/>
   </bookViews>
   <sheets>
     <sheet name="petals" sheetId="5" r:id="rId1"/>
@@ -1902,12 +1902,6 @@
     <t>991915</t>
   </si>
   <si>
-    <t> 8D7CB8</t>
-  </si>
-  <si>
-    <t> 729BD2</t>
-  </si>
-  <si>
     <t>Finance Change Elsewhere</t>
   </si>
   <si>
@@ -2113,6 +2107,12 @@
   </si>
   <si>
     <t>'@offset.svg</t>
+  </si>
+  <si>
+    <t>8D7CB8</t>
+  </si>
+  <si>
+    <t>729BD2</t>
   </si>
 </sst>
 </file>
@@ -3495,8 +3495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C1FEF7-6E5A-4A37-95FB-97DB96CB71EA}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3767,7 +3767,7 @@
         <v>484</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>494</v>
+        <v>563</v>
       </c>
       <c r="G10" s="43" t="s">
         <v>471</v>
@@ -3794,7 +3794,7 @@
         <v>485</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>495</v>
+        <v>564</v>
       </c>
       <c r="G11" s="43" t="s">
         <v>471</v>
@@ -4403,7 +4403,7 @@
         <v>444</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H2" s="40" t="s">
         <v>301</v>
@@ -4429,7 +4429,7 @@
         <v>445</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>301</v>
@@ -4455,7 +4455,7 @@
         <v>446</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H4" s="40" t="s">
         <v>301</v>
@@ -4481,7 +4481,7 @@
         <v>447</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>302</v>
@@ -4507,7 +4507,7 @@
         <v>448</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H6" s="40" t="s">
         <v>302</v>
@@ -4518,7 +4518,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -4533,7 +4533,7 @@
         <v>449</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H7" s="40" t="s">
         <v>307</v>
@@ -4601,7 +4601,7 @@
         <v>451</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -4621,7 +4621,7 @@
         <v>453</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4641,7 +4641,7 @@
         <v>452</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -4661,7 +4661,7 @@
         <v>454</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -4892,16 +4892,16 @@
         <v>#N/A</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W2" s="15"/>
       <c r="Z2" s="5"/>
@@ -4963,10 +4963,10 @@
         <v>331</v>
       </c>
       <c r="S3" s="31" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="U3" s="7">
         <v>5</v>
@@ -5038,10 +5038,10 @@
         <v>331</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U4" s="7">
         <v>3</v>
@@ -5103,16 +5103,16 @@
         <v>331</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W5" s="15" t="s">
         <v>410</v>
@@ -5178,10 +5178,10 @@
         <v>333</v>
       </c>
       <c r="S6" s="31" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U6" s="7">
         <v>2</v>
@@ -5253,10 +5253,10 @@
         <v>333</v>
       </c>
       <c r="S7" s="31" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U7" s="7">
         <v>2</v>
@@ -5328,10 +5328,10 @@
         <v>333</v>
       </c>
       <c r="S8" s="31" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U8" s="7">
         <v>2</v>
@@ -5405,10 +5405,10 @@
         <v>333</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U9" s="7">
         <v>3</v>
@@ -5476,10 +5476,10 @@
         <v>333</v>
       </c>
       <c r="S10" s="31" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U10" s="7">
         <v>2</v>
@@ -5544,13 +5544,13 @@
         <v>333</v>
       </c>
       <c r="S11" s="31" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V11" s="7">
         <v>1</v>
@@ -5619,10 +5619,10 @@
         <v>333</v>
       </c>
       <c r="S12" s="31" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U12" s="7">
         <v>2</v>
@@ -5692,10 +5692,10 @@
         <v>333</v>
       </c>
       <c r="S13" s="31" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U13" s="7">
         <v>4</v>
@@ -5765,10 +5765,10 @@
         <v>333</v>
       </c>
       <c r="S14" s="31" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U14" s="7">
         <v>4</v>
@@ -5838,10 +5838,10 @@
         <v>333</v>
       </c>
       <c r="S15" s="31" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U15" s="7">
         <v>4</v>
@@ -5913,10 +5913,10 @@
         <v>333</v>
       </c>
       <c r="S16" s="31" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U16" s="7">
         <v>2</v>
@@ -5980,16 +5980,16 @@
         <v>333</v>
       </c>
       <c r="S17" s="31" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W17" s="15"/>
       <c r="Z17" s="5"/>
@@ -6051,10 +6051,10 @@
         <v>333</v>
       </c>
       <c r="S18" s="31" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U18" s="7">
         <v>4</v>
@@ -6122,10 +6122,10 @@
         <v>333</v>
       </c>
       <c r="S19" s="31" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U19" s="7">
         <v>4</v>
@@ -6193,10 +6193,10 @@
         <v>333</v>
       </c>
       <c r="S20" s="31" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U20" s="7">
         <v>2</v>
@@ -6260,16 +6260,16 @@
         <v>331</v>
       </c>
       <c r="S21" s="31" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W21" s="15"/>
       <c r="Z21" s="5"/>
@@ -6327,16 +6327,16 @@
         <v>331</v>
       </c>
       <c r="S22" s="31" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V22" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W22" s="15" t="s">
         <v>418</v>
@@ -6396,16 +6396,16 @@
         <v>331</v>
       </c>
       <c r="S23" s="31" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W23" s="15" t="s">
         <v>419</v>
@@ -6463,16 +6463,16 @@
         <v>331</v>
       </c>
       <c r="S24" s="31" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U24" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V24" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W24" s="15"/>
       <c r="Z24" s="5"/>
@@ -6534,10 +6534,10 @@
         <v>331</v>
       </c>
       <c r="S25" s="31" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U25" s="7">
         <v>3</v>
@@ -6609,10 +6609,10 @@
         <v>332</v>
       </c>
       <c r="S26" s="31" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="U26" s="7">
         <v>1</v>
@@ -6682,10 +6682,10 @@
         <v>332</v>
       </c>
       <c r="S27" s="31" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="U27" s="7">
         <v>1</v>
@@ -6757,10 +6757,10 @@
         <v>332</v>
       </c>
       <c r="S28" s="31" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="U28" s="7">
         <v>1</v>
@@ -6830,10 +6830,10 @@
         <v>332</v>
       </c>
       <c r="S29" s="31" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U29" s="7">
         <v>2</v>
@@ -6903,10 +6903,10 @@
         <v>332</v>
       </c>
       <c r="S30" s="31" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U30" s="7">
         <v>2</v>
@@ -6976,10 +6976,10 @@
         <v>332</v>
       </c>
       <c r="S31" s="31" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U31" s="7">
         <v>2</v>
@@ -7051,10 +7051,10 @@
         <v>332</v>
       </c>
       <c r="S32" s="31" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U32" s="7">
         <v>2</v>
@@ -7128,10 +7128,10 @@
         <v>332</v>
       </c>
       <c r="S33" s="31" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U33" s="7">
         <v>2</v>
@@ -7203,10 +7203,10 @@
         <v>332</v>
       </c>
       <c r="S34" s="31" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="U34" s="7">
         <v>1</v>
@@ -7278,10 +7278,10 @@
         <v>332</v>
       </c>
       <c r="S35" s="31" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U35" s="7">
         <v>2</v>
@@ -7351,10 +7351,10 @@
         <v>332</v>
       </c>
       <c r="S36" s="31" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U36" s="7">
         <v>3</v>
@@ -7426,10 +7426,10 @@
         <v>332</v>
       </c>
       <c r="S37" s="31" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U37" s="7">
         <v>2</v>
@@ -7501,10 +7501,10 @@
         <v>332</v>
       </c>
       <c r="S38" s="31" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U38" s="7">
         <v>2</v>
@@ -7572,10 +7572,10 @@
         <v>332</v>
       </c>
       <c r="S39" s="31" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U39" s="7">
         <v>3</v>
@@ -7647,10 +7647,10 @@
         <v>332</v>
       </c>
       <c r="S40" s="31" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U40" s="7">
         <v>3</v>
@@ -7720,10 +7720,10 @@
         <v>332</v>
       </c>
       <c r="S41" s="31" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U41" s="7">
         <v>2</v>
@@ -7795,10 +7795,10 @@
         <v>332</v>
       </c>
       <c r="S42" s="31" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U42" s="7">
         <v>2</v>
@@ -7868,10 +7868,10 @@
         <v>332</v>
       </c>
       <c r="S43" s="31" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U43" s="7">
         <v>3</v>
@@ -7941,10 +7941,10 @@
         <v>332</v>
       </c>
       <c r="S44" s="31" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="T44" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U44" s="7">
         <v>2</v>
@@ -8012,10 +8012,10 @@
         <v>332</v>
       </c>
       <c r="S45" s="31" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="T45" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U45" s="7">
         <v>3</v>
@@ -8083,10 +8083,10 @@
         <v>334</v>
       </c>
       <c r="S46" s="31" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="T46" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="U46" s="7">
         <v>5</v>
@@ -8154,10 +8154,10 @@
         <v>334</v>
       </c>
       <c r="S47" s="31" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="T47" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U47" s="7">
         <v>3</v>
@@ -8227,10 +8227,10 @@
         <v>334</v>
       </c>
       <c r="S48" s="31" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="U48" s="7">
         <v>5</v>
@@ -8299,10 +8299,10 @@
         <v>334</v>
       </c>
       <c r="S49" s="31" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U49" s="7">
         <v>3</v>
@@ -8366,16 +8366,16 @@
         <v>334</v>
       </c>
       <c r="S50" s="31" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W50" s="15"/>
       <c r="Z50" s="5"/>
@@ -8437,10 +8437,10 @@
         <v>335</v>
       </c>
       <c r="S51" s="31" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="T51" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="U51" s="7">
         <v>5</v>
@@ -8501,16 +8501,16 @@
         <v>#N/A</v>
       </c>
       <c r="S52" s="31" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="T52" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U52" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W52" s="15" t="s">
         <v>430</v>
@@ -8565,19 +8565,19 @@
         <v>352</v>
       </c>
       <c r="R53" s="31" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="S53" s="31" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="T53" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="U53" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V53" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W53" s="15" t="s">
         <v>432</v>
@@ -8608,7 +8608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EB303B-3C82-4D29-A5F6-85FF930F1102}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -9207,6 +9207,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2e6c9e18-af56-461d-b5b1-9da131569893">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="df906139-7fd4-4cb3-8d03-9354f4288e29" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010089919C7F80A1924CB02BF4AF797918CA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="758f151e4d62a3f26d649962cff62c70">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e6c9e18-af56-461d-b5b1-9da131569893" xmlns:ns3="df906139-7fd4-4cb3-8d03-9354f4288e29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c25e2c4c4b3b3c9448ba0bace908713c" ns2:_="" ns3:_="">
     <xsd:import namespace="2e6c9e18-af56-461d-b5b1-9da131569893"/>
@@ -9437,27 +9457,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52915743-EE36-4F2E-992B-AE08EE0CC029}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2e6c9e18-af56-461d-b5b1-9da131569893"/>
+    <ds:schemaRef ds:uri="df906139-7fd4-4cb3-8d03-9354f4288e29"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2e6c9e18-af56-461d-b5b1-9da131569893">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="df906139-7fd4-4cb3-8d03-9354f4288e29" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFCB6F13-4F8A-46A9-8AFE-9B971252E381}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC3F18F1-0720-4210-BB55-68E03E48B30C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9474,23 +9493,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFCB6F13-4F8A-46A9-8AFE-9B971252E381}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52915743-EE36-4F2E-992B-AE08EE0CC029}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2e6c9e18-af56-461d-b5b1-9da131569893"/>
-    <ds:schemaRef ds:uri="df906139-7fd4-4cb3-8d03-9354f4288e29"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
some improvements in look to show items in grids; spacing not yet right
</commit_message>
<xml_diff>
--- a/aux/master-spreadsheet.xlsx
+++ b/aux/master-spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\09_next_projects\SEC\SEC-card-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60787291-3D14-4787-93DB-56853B61ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B05D2F-2D29-4E8F-8A6A-B7AF6735612C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8231788-E26F-497A-84D5-4BB029B3585E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F8231788-E26F-497A-84D5-4BB029B3585E}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="12" r:id="rId1"/>
@@ -463,7 +463,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="891">
   <si>
     <t>Big heating changes</t>
   </si>
@@ -2070,9 +2070,6 @@
     <t>See if there are local environmental initiatives promoting biodiversity  that you can be linked to, particularly if you are a charge without grounds of your own (e.g. the local council - could you or a group manage an area of their grounds,  a local litter picking group)</t>
   </si>
   <si>
-    <t>Partner with local intiatives</t>
-  </si>
-  <si>
     <t>T3.02</t>
   </si>
   <si>
@@ -2445,9 +2442,6 @@
     <t>T4.05</t>
   </si>
   <si>
-    <t>Where appropriate, normalise meetings online, recognizing the need to balance this with in-person meetings to ensure flourishing of people and communities. Note: online platforms are no panacea, and tools such as Zoom/Microsoft Teams increase carbon footprint, especially with video enabled.</t>
-  </si>
-  <si>
     <t>https://energysavingtrust.org.uk/advice/buying-a-second-hand-electric-car-or-van/</t>
   </si>
   <si>
@@ -2730,9 +2724,6 @@
     <t>T9.07</t>
   </si>
   <si>
-    <t>Apply for financial support from the Provincial Buildings Committee grant fund, clearly demonstrating the carbon savings from each element of your application. PLEASE NOTE: further guidance and criteria regarding the Net Zero related applications will be provided soon.</t>
-  </si>
-  <si>
     <t>Apply to the SEC Provincial Buildings Committee Grant fund</t>
   </si>
   <si>
@@ -2775,10 +2766,6 @@
     <t>Form an eco-group in your church as a starting point to discuss this toolkit and to engage with the Diocesan Eco Group and the SEC over the longer term</t>
   </si>
   <si>
-    <t>Engage with other churches, ecumenical partners, interfaith groups,  and local community groups on climate issues; explore how you might work together, share skills and encourage one another. Youth groups and community groups (e.g local parks, offering things in the local parks for others rather than just in our churches)
-Church In Society will provide support to enable engagement with schools and care homes on these issues</t>
-  </si>
-  <si>
     <t xml:space="preserve">Promote local environmental initiatives through the church magazine, posters, notices, and prayer. </t>
   </si>
   <si>
@@ -3131,13 +3118,31 @@
   </si>
   <si>
     <t>quote_word_count</t>
+  </si>
+  <si>
+    <t>Partner with local initiatives</t>
+  </si>
+  <si>
+    <t>T8.07</t>
+  </si>
+  <si>
+    <t>T8.08</t>
+  </si>
+  <si>
+    <t>Where appropriate, normalise meetings online, recognizing the need to balance this with in-person meetings to ensure flourishing of people and communities. Note that online platforms are no panacea, and tools such as Zoom/Microsoft Teams increase carbon footprint, especially with video enabled.</t>
+  </si>
+  <si>
+    <t>Apply for financial support from the Provincial Buildings Committee grant fund, clearly demonstrating the carbon savings from each element of your application. PLEASE NOTE that further guidance and criteria regarding the Net Zero related applications will be provided soon.</t>
+  </si>
+  <si>
+    <t>Engage with other churches, ecumenical partners, interfaith groups,  and local community groups on climate issues; explore how you might work together, share skills and encourage one another. Youth groups and community groups (e.g local parks, offering things in the local parks for others rather than just in our churches). &lt;br&gt;Church In Society will provide support to enable engagement with schools and care homes on these issues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3309,11 +3314,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3589,26 +3589,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3698,6 +3678,26 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -4065,6 +4065,12 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>Don't use new lines in any of the cells - instead put &lt;br&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
@@ -4174,7 +4180,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>- two tasks missing numbers</a:t>
+            <a:t>- two tasks missing numbers - JC has assigned, RW can reassign.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4610,13 +4616,13 @@
     <tableColumn id="12" xr3:uid="{FA55F699-84E1-4B25-BA0E-9FAE66964DE4}" name="carbon_number" dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(K2),"",LEN(Table5[[#This Row],[carbon_stars]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FDCB454F-7833-4325-A435-6B1684500B5F}" name="description_word_count" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{FDCB454F-7833-4325-A435-6B1684500B5F}" name="description_word_count" dataDxfId="18">
       <calculatedColumnFormula>LEN(H2)-LEN(SUBSTITUTE(H2," ",""))+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D181305-4EF9-45D6-BF2C-20D2F725CE20}" name="quote_word_count" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{0D181305-4EF9-45D6-BF2C-20D2F725CE20}" name="quote_word_count" dataDxfId="17">
       <calculatedColumnFormula>LEN(I2)-LEN(SUBSTITUTE(I2," ",""))+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F0CBB9BB-6230-4245-9C7B-91036CD196E2}" name="more_quotes" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{F0CBB9BB-6230-4245-9C7B-91036CD196E2}" name="more_quotes" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4672,24 +4678,24 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{963A35FE-C41F-4284-9822-DF29E5123E22}" name="Table57" displayName="Table57" ref="A1:L13" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{963A35FE-C41F-4284-9822-DF29E5123E22}" name="Table57" displayName="Table57" ref="A1:L13" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:L13" xr:uid="{7098ABA5-EA9C-4D71-BC01-3BB0F24D806D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L13">
     <sortCondition ref="I1:I13"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="13" xr3:uid="{F3C35260-48C2-40E3-8688-849B947E5ECF}" name="For localised or space heating?" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{D30B0BCF-7DDA-416D-BBBE-D32FDD46F58E}" name="New card title" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{F99FBD27-1C5E-402C-A616-F45E2E26FAF0}" name="New category" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{A76E63D5-BC50-4C67-B842-47972BCED705}" name="SEC target area" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{3BC6CF9D-EE37-48DB-B02E-5467E98B86BC}" name="100 words" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{7DBFEED5-7FA1-436E-B3DA-FB5479FD7033}" name="25 word motivation" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{5C1D7DE1-A381-4A64-A886-D280AB27C207}" name="carbon stars" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{55F12E45-C916-4681-AD33-33668A50D812}" name="cost" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{055DB5D1-F8AF-4922-9187-ED95D7516444}" name="Status" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{CA2BCA4F-75E4-4BB2-BAAC-22224C509701}" name="Old category" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{23D8D185-2D8D-46AA-B9CE-CD715024BFAE}" name="Old card title" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{2F2D8AD0-0847-4F9D-BAB9-DEB95ED5A68A}" name="print form of cost" dataDxfId="4">
+    <tableColumn id="13" xr3:uid="{F3C35260-48C2-40E3-8688-849B947E5ECF}" name="For localised or space heating?" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{D30B0BCF-7DDA-416D-BBBE-D32FDD46F58E}" name="New card title" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{F99FBD27-1C5E-402C-A616-F45E2E26FAF0}" name="New category" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A76E63D5-BC50-4C67-B842-47972BCED705}" name="SEC target area" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{3BC6CF9D-EE37-48DB-B02E-5467E98B86BC}" name="100 words" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{7DBFEED5-7FA1-436E-B3DA-FB5479FD7033}" name="25 word motivation" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{5C1D7DE1-A381-4A64-A886-D280AB27C207}" name="carbon stars" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{55F12E45-C916-4681-AD33-33668A50D812}" name="cost" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{055DB5D1-F8AF-4922-9187-ED95D7516444}" name="Status" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{CA2BCA4F-75E4-4BB2-BAAC-22224C509701}" name="Old category" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{23D8D185-2D8D-46AA-B9CE-CD715024BFAE}" name="Old card title" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{2F2D8AD0-0847-4F9D-BAB9-DEB95ED5A68A}" name="print form of cost" dataDxfId="2">
       <calculatedColumnFormula>IF(H2="£",1,(IF(H2="££",2,IF(H2="£££",3,IF(H2="££££",4,IF(H2="£££££",5,IF(H2="?","?")))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5123,7 +5129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01D17A7-7725-4BF6-96D1-5F3A71A49F3E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
@@ -5856,8 +5862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1AF78F-40C0-470E-9E76-7A81EC96B5A7}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6200,7 +6206,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>535</v>
+        <v>885</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>534</v>
@@ -6211,16 +6217,16 @@
     </row>
     <row r="18" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B18" s="60">
         <v>31</v>
       </c>
       <c r="C18" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>537</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>538</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>255</v>
@@ -6228,16 +6234,16 @@
     </row>
     <row r="19" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B19" s="60">
         <v>32</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>255</v>
@@ -6245,16 +6251,16 @@
     </row>
     <row r="20" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B20" s="60">
         <v>33</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>255</v>
@@ -6262,16 +6268,16 @@
     </row>
     <row r="21" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B21" s="60">
         <v>34</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>255</v>
@@ -6279,16 +6285,16 @@
     </row>
     <row r="22" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B22" s="60">
         <v>35</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>255</v>
@@ -6296,16 +6302,16 @@
     </row>
     <row r="23" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B23" s="60">
         <v>40</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>264</v>
@@ -6313,16 +6319,16 @@
     </row>
     <row r="24" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="32" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B24" s="60">
         <v>41</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>264</v>
@@ -6330,16 +6336,16 @@
     </row>
     <row r="25" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="32" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B25" s="60">
         <v>42</v>
       </c>
       <c r="C25" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>654</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>655</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>264</v>
@@ -6347,16 +6353,16 @@
     </row>
     <row r="26" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="32" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B26" s="60">
         <v>43</v>
       </c>
       <c r="C26" s="23" t="s">
+        <v>656</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>657</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>658</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>264</v>
@@ -6364,16 +6370,16 @@
     </row>
     <row r="27" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B27" s="60">
         <v>44</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>660</v>
+        <v>888</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>264</v>
@@ -6381,16 +6387,16 @@
     </row>
     <row r="28" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="32" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B28" s="60">
         <v>50</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>265</v>
@@ -6398,16 +6404,16 @@
     </row>
     <row r="29" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="32" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B29" s="60">
         <v>51</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>265</v>
@@ -6415,16 +6421,16 @@
     </row>
     <row r="30" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B30" s="60">
         <v>52</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="E30" s="23" t="s">
         <v>265</v>
@@ -6432,16 +6438,16 @@
     </row>
     <row r="31" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="32" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B31" s="60">
         <v>53</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>265</v>
@@ -6449,16 +6455,16 @@
     </row>
     <row r="32" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B32" s="60">
         <v>54</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>265</v>
@@ -6466,16 +6472,16 @@
     </row>
     <row r="33" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="32" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B33" s="60">
         <v>60</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E33" s="23" t="s">
         <v>256</v>
@@ -6483,16 +6489,16 @@
     </row>
     <row r="34" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="32" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B34" s="60">
         <v>61</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E34" s="23" t="s">
         <v>256</v>
@@ -6500,16 +6506,16 @@
     </row>
     <row r="35" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="32" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B35" s="60">
         <v>62</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>256</v>
@@ -6517,16 +6523,16 @@
     </row>
     <row r="36" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="32" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B36" s="60">
         <v>63</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E36" s="23" t="s">
         <v>256</v>
@@ -6534,16 +6540,16 @@
     </row>
     <row r="37" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="32" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B37" s="60">
         <v>70</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>257</v>
@@ -6551,16 +6557,16 @@
     </row>
     <row r="38" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B38" s="60">
         <v>71</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>257</v>
@@ -6568,16 +6574,16 @@
     </row>
     <row r="39" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="B39" s="60">
         <v>71</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="E39" s="23" t="s">
         <v>257</v>
@@ -6585,16 +6591,16 @@
     </row>
     <row r="40" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B40" s="60">
         <v>72</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E40" s="23" t="s">
         <v>257</v>
@@ -6602,44 +6608,50 @@
     </row>
     <row r="41" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="32" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B41" s="60">
         <v>80</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="32"/>
-      <c r="B42" s="60"/>
+      <c r="A42" s="32" t="s">
+        <v>887</v>
+      </c>
+      <c r="B42" s="60">
+        <v>85.2</v>
+      </c>
       <c r="C42" s="23" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>847</v>
-      </c>
-      <c r="E42" s="23"/>
+        <v>843</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B43" s="60">
         <v>81</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="E43" s="23" t="s">
         <v>258</v>
@@ -6647,16 +6659,16 @@
     </row>
     <row r="44" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B44" s="60">
         <v>82</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>258</v>
@@ -6664,16 +6676,16 @@
     </row>
     <row r="45" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="32" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B45" s="60">
         <v>83</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="E45" s="23" t="s">
         <v>258</v>
@@ -6681,16 +6693,16 @@
     </row>
     <row r="46" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="32" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B46" s="60">
         <v>84</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E46" s="23" t="s">
         <v>258</v>
@@ -6698,29 +6710,33 @@
     </row>
     <row r="47" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="32" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B47" s="60">
         <v>85</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="E47" s="23" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="94" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
-      <c r="B48" s="60"/>
+      <c r="A48" s="32" t="s">
+        <v>886</v>
+      </c>
+      <c r="B48" s="60">
+        <v>85.1</v>
+      </c>
       <c r="C48" s="23" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>258</v>
@@ -6734,10 +6750,10 @@
         <v>86</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E49" s="23" t="s">
         <v>259</v>
@@ -6745,16 +6761,16 @@
     </row>
     <row r="50" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B50" s="60">
         <v>87</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E50" s="23" t="s">
         <v>259</v>
@@ -6771,7 +6787,7 @@
         <v>302</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E51" s="23" t="s">
         <v>259</v>
@@ -6779,16 +6795,16 @@
     </row>
     <row r="52" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B52" s="60">
         <v>89</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E52" s="23" t="s">
         <v>259</v>
@@ -6796,16 +6812,16 @@
     </row>
     <row r="53" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B53" s="60">
         <v>90</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E53" s="23" t="s">
         <v>259</v>
@@ -6813,16 +6829,16 @@
     </row>
     <row r="54" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="32" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B54" s="60">
         <v>91</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E54" s="23" t="s">
         <v>259</v>
@@ -6830,16 +6846,16 @@
     </row>
     <row r="55" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="32" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B55" s="60">
         <v>92</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>755</v>
+        <v>889</v>
       </c>
       <c r="E55" s="23" t="s">
         <v>259</v>
@@ -6847,16 +6863,16 @@
     </row>
     <row r="56" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="32" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B56" s="60">
         <v>100</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E56" t="s">
         <v>260</v>
@@ -6864,33 +6880,33 @@
     </row>
     <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="32" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B57" s="60">
         <v>101</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="E57" s="23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="32" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B58" s="60">
         <v>102</v>
       </c>
       <c r="C58" s="61" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>770</v>
+        <v>890</v>
       </c>
       <c r="E58" t="s">
         <v>260</v>
@@ -6899,16 +6915,16 @@
     </row>
     <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="32" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="B59" s="60">
         <v>103</v>
       </c>
       <c r="C59" s="61" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="E59" s="23" t="s">
         <v>260</v>
@@ -6916,16 +6932,16 @@
     </row>
     <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="32" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="B60" s="60">
         <v>104</v>
       </c>
       <c r="C60" s="61" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="E60" t="s">
         <v>260</v>
@@ -6933,16 +6949,16 @@
     </row>
     <row r="61" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="32" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B61" s="60">
         <v>105</v>
       </c>
       <c r="C61" s="61" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>260</v>
@@ -6950,16 +6966,16 @@
     </row>
     <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="32" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B62" s="60">
         <v>106</v>
       </c>
       <c r="C62" s="61" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="E62" t="s">
         <v>260</v>
@@ -7004,7 +7020,7 @@
   <dimension ref="A1:AM54"/>
   <sheetViews>
     <sheetView zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7094,10 +7110,10 @@
         <v>412</v>
       </c>
       <c r="P1" s="45" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="Q1" s="45" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="R1" s="46" t="s">
         <v>241</v>
@@ -7126,7 +7142,7 @@
         <v>309</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>117</v>
@@ -7191,7 +7207,7 @@
         <v>310</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>118</v>
@@ -7301,7 +7317,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>253</v>
@@ -7316,7 +7332,7 @@
         <v>327</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>232</v>
@@ -7376,7 +7392,7 @@
         <v>328</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>500</v>
@@ -7500,7 +7516,7 @@
         <v>330</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>370</v>
@@ -7558,7 +7574,7 @@
         <v>331</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>371</v>
@@ -7931,7 +7947,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>253</v>
@@ -7946,7 +7962,7 @@
         <v>337</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>129</v>
@@ -8531,7 +8547,7 @@
         <v>346</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>137</v>
@@ -8596,7 +8612,7 @@
         <v>347</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>138</v>
@@ -8728,7 +8744,7 @@
         <v>349</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>140</v>
@@ -9049,7 +9065,7 @@
         <v>314</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>121</v>
@@ -9116,7 +9132,7 @@
         <v>315</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>122</v>
@@ -9181,7 +9197,7 @@
         <v>316</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>231</v>
@@ -9244,7 +9260,7 @@
         <v>317</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>123</v>
@@ -9304,7 +9320,7 @@
         <v>318</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>124</v>
@@ -9495,7 +9511,7 @@
         <v>321</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I39" s="27" t="s">
         <v>364</v>
@@ -9558,7 +9574,7 @@
         <v>322</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>365</v>
@@ -9809,7 +9825,7 @@
         <v>326</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>367</v>
@@ -9935,7 +9951,7 @@
         <v>353</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>143</v>
@@ -9998,7 +10014,7 @@
         <v>354</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>496</v>
@@ -10308,7 +10324,7 @@
         <v>359</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>381</v>
@@ -10853,13 +10869,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
+        <v>550</v>
+      </c>
+      <c r="B12" t="s">
         <v>551</v>
       </c>
-      <c r="B12" t="s">
-        <v>552</v>
-      </c>
       <c r="C12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D12" t="s">
         <v>255</v>
@@ -10867,13 +10883,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="B13" t="s">
         <v>553</v>
       </c>
-      <c r="B13" t="s">
-        <v>554</v>
-      </c>
       <c r="C13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D13" t="s">
         <v>255</v>
@@ -10881,13 +10897,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="B14" t="s">
         <v>555</v>
       </c>
-      <c r="B14" t="s">
-        <v>556</v>
-      </c>
       <c r="C14" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D14" t="s">
         <v>255</v>
@@ -10895,41 +10911,41 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="B15" t="s">
         <v>557</v>
       </c>
-      <c r="B15" t="s">
-        <v>558</v>
-      </c>
       <c r="C15" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B16" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C16" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E16" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="B17" t="s">
         <v>560</v>
       </c>
-      <c r="B17" t="s">
-        <v>561</v>
-      </c>
       <c r="C17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D17" t="s">
         <v>255</v>
@@ -10937,13 +10953,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="B18" t="s">
         <v>562</v>
       </c>
-      <c r="B18" t="s">
-        <v>563</v>
-      </c>
       <c r="C18" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D18" t="s">
         <v>260</v>
@@ -10951,13 +10967,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="B19" t="s">
         <v>569</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>570</v>
-      </c>
-      <c r="C19" t="s">
-        <v>571</v>
       </c>
       <c r="F19" t="s">
         <v>86</v>
@@ -10965,10 +10981,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="B20" t="s">
         <v>572</v>
-      </c>
-      <c r="B20" t="s">
-        <v>573</v>
       </c>
       <c r="F20" t="s">
         <v>93</v>
@@ -10976,13 +10992,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="B21" t="s">
         <v>574</v>
       </c>
-      <c r="B21" t="s">
-        <v>575</v>
-      </c>
       <c r="C21" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E21" t="s">
         <v>288</v>
@@ -10993,13 +11009,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
+        <v>593</v>
+      </c>
+      <c r="B22" t="s">
         <v>594</v>
       </c>
-      <c r="B22" t="s">
-        <v>595</v>
-      </c>
       <c r="C22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D22" t="s">
         <v>253</v>
@@ -11010,13 +11026,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="B23" t="s">
+        <v>882</v>
+      </c>
+      <c r="C23" t="s">
         <v>596</v>
-      </c>
-      <c r="B23" t="s">
-        <v>886</v>
-      </c>
-      <c r="C23" t="s">
-        <v>597</v>
       </c>
       <c r="D23" t="s">
         <v>253</v>
@@ -11027,13 +11043,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C24" t="s">
         <v>598</v>
-      </c>
-      <c r="C24" t="s">
-        <v>599</v>
       </c>
       <c r="D24" t="s">
         <v>253</v>
@@ -11041,13 +11057,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B25" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C25" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E25" t="s">
         <v>296</v>
@@ -11055,13 +11071,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
+        <v>601</v>
+      </c>
+      <c r="B26" t="s">
+        <v>876</v>
+      </c>
+      <c r="C26" t="s">
         <v>602</v>
-      </c>
-      <c r="B26" t="s">
-        <v>880</v>
-      </c>
-      <c r="C26" t="s">
-        <v>603</v>
       </c>
       <c r="D26" t="s">
         <v>253</v>
@@ -11072,13 +11088,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B27" t="s">
+        <v>603</v>
+      </c>
+      <c r="C27" t="s">
         <v>604</v>
-      </c>
-      <c r="C27" t="s">
-        <v>605</v>
       </c>
       <c r="E27" t="s">
         <v>286</v>
@@ -11086,13 +11102,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
+        <v>606</v>
+      </c>
+      <c r="B28" t="s">
         <v>607</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>608</v>
-      </c>
-      <c r="C28" t="s">
-        <v>609</v>
       </c>
       <c r="D28" t="s">
         <v>253</v>
@@ -11100,13 +11116,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B29" t="s">
+        <v>609</v>
+      </c>
+      <c r="C29" t="s">
         <v>610</v>
-      </c>
-      <c r="C29" t="s">
-        <v>611</v>
       </c>
       <c r="D29" t="s">
         <v>253</v>
@@ -11114,13 +11130,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B30" t="s">
+        <v>612</v>
+      </c>
+      <c r="C30" t="s">
         <v>613</v>
-      </c>
-      <c r="C30" t="s">
-        <v>614</v>
       </c>
       <c r="D30" t="s">
         <v>253</v>
@@ -11131,13 +11147,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="19" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B31" t="s">
+        <v>615</v>
+      </c>
+      <c r="C31" t="s">
         <v>616</v>
-      </c>
-      <c r="C31" t="s">
-        <v>617</v>
       </c>
       <c r="D31" t="s">
         <v>253</v>
@@ -11148,13 +11164,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="B32" t="s">
         <v>619</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>620</v>
-      </c>
-      <c r="C32" t="s">
-        <v>621</v>
       </c>
       <c r="D32" t="s">
         <v>254</v>
@@ -11165,13 +11181,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B33" t="s">
+        <v>621</v>
+      </c>
+      <c r="C33" t="s">
         <v>622</v>
-      </c>
-      <c r="C33" t="s">
-        <v>623</v>
       </c>
       <c r="D33" t="s">
         <v>254</v>
@@ -11182,13 +11198,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B34" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="C34" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D34" t="s">
         <v>254</v>
@@ -11199,13 +11215,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="19" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B35" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C35" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D35" t="s">
         <v>254</v>
@@ -11216,13 +11232,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="19" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B36" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C36" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D36" t="s">
         <v>254</v>
@@ -11233,13 +11249,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B37" t="s">
+        <v>628</v>
+      </c>
+      <c r="C37" t="s">
         <v>629</v>
-      </c>
-      <c r="C37" t="s">
-        <v>630</v>
       </c>
       <c r="D37" t="s">
         <v>254</v>
@@ -11250,13 +11266,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="19" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B38" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C38" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D38" t="s">
         <v>254</v>
@@ -11267,13 +11283,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B39" t="s">
+        <v>632</v>
+      </c>
+      <c r="C39" t="s">
         <v>633</v>
-      </c>
-      <c r="C39" t="s">
-        <v>634</v>
       </c>
       <c r="D39" t="s">
         <v>254</v>
@@ -11284,13 +11300,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B40" t="s">
+        <v>635</v>
+      </c>
+      <c r="C40" t="s">
         <v>636</v>
-      </c>
-      <c r="C40" t="s">
-        <v>637</v>
       </c>
       <c r="D40" t="s">
         <v>254</v>
@@ -11301,13 +11317,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="19" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B41" t="s">
+        <v>638</v>
+      </c>
+      <c r="C41" t="s">
         <v>639</v>
-      </c>
-      <c r="C41" t="s">
-        <v>640</v>
       </c>
       <c r="D41" t="s">
         <v>254</v>
@@ -11318,10 +11334,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="19" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B42" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D42" t="s">
         <v>254</v>
@@ -11329,13 +11345,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B43" t="s">
+        <v>644</v>
+      </c>
+      <c r="C43" t="s">
         <v>645</v>
-      </c>
-      <c r="C43" t="s">
-        <v>646</v>
       </c>
       <c r="D43" t="s">
         <v>264</v>
@@ -11343,13 +11359,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B44" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C44" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="D44" t="s">
         <v>264</v>
@@ -11357,13 +11373,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="19" t="s">
+        <v>661</v>
+      </c>
+      <c r="B45" t="s">
+        <v>662</v>
+      </c>
+      <c r="C45" t="s">
         <v>663</v>
-      </c>
-      <c r="B45" t="s">
-        <v>664</v>
-      </c>
-      <c r="C45" t="s">
-        <v>665</v>
       </c>
       <c r="D45" t="s">
         <v>264</v>
@@ -11371,13 +11387,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B46" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C46" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D46" t="s">
         <v>265</v>
@@ -11385,13 +11401,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="19" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B47" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C47" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D47" t="s">
         <v>265</v>
@@ -11399,13 +11415,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="19" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B48" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C48" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D48" t="s">
         <v>265</v>
@@ -11413,13 +11429,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
+        <v>700</v>
+      </c>
+      <c r="B49" t="s">
+        <v>701</v>
+      </c>
+      <c r="C49" t="s">
         <v>702</v>
-      </c>
-      <c r="B49" t="s">
-        <v>703</v>
-      </c>
-      <c r="C49" t="s">
-        <v>704</v>
       </c>
       <c r="D49" t="s">
         <v>257</v>
@@ -11427,13 +11443,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B50" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C50" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D50" t="s">
         <v>257</v>
@@ -11441,13 +11457,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B51" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C51" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D51" t="s">
         <v>257</v>
@@ -11455,13 +11471,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="19" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B52" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C52" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D52" t="s">
         <v>257</v>
@@ -11469,30 +11485,30 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="19" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B53" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C53" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D53" t="s">
         <v>258</v>
       </c>
       <c r="E53" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="19" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B54" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C54" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D54" t="s">
         <v>258</v>
@@ -11500,47 +11516,47 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="19" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B55" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="C55" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D55" t="s">
         <v>258</v>
       </c>
       <c r="E55" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="19" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B56" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C56" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D56" t="s">
         <v>258</v>
       </c>
       <c r="E56" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="B57" t="s">
+        <v>732</v>
+      </c>
+      <c r="C57" t="s">
         <v>733</v>
-      </c>
-      <c r="B57" t="s">
-        <v>734</v>
-      </c>
-      <c r="C57" t="s">
-        <v>735</v>
       </c>
       <c r="D57" t="s">
         <v>258</v>
@@ -11548,13 +11564,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="B58" t="s">
         <v>740</v>
       </c>
-      <c r="B58" t="s">
-        <v>742</v>
-      </c>
       <c r="C58" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D58" t="s">
         <v>259</v>
@@ -11562,13 +11578,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="B59" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="C59" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D59" t="s">
         <v>259</v>
@@ -11576,13 +11592,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="19" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B60" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C60" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D60" t="s">
         <v>260</v>
@@ -11590,30 +11606,30 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="19" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="B61" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C61" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D61" t="s">
         <v>260</v>
       </c>
       <c r="E61" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="19" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B62" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C62" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D62" t="s">
         <v>257</v>
@@ -11621,30 +11637,30 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="19" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="B63" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C63" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D63" t="s">
         <v>259</v>
       </c>
       <c r="E63" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="19" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B64" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C64" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D64" t="s">
         <v>259</v>
@@ -11655,13 +11671,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="19" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="B65" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C65" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D65" t="s">
         <v>259</v>
@@ -11672,19 +11688,19 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="19" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B66" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C66" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D66" t="s">
         <v>259</v>
       </c>
       <c r="E66" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -11692,27 +11708,27 @@
         <v>449</v>
       </c>
       <c r="B67" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C67" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D67" t="s">
         <v>259</v>
       </c>
       <c r="E67" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="19" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="B68" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="C68" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D68" t="s">
         <v>260</v>
@@ -11720,13 +11736,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="19" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B69" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C69" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D69" t="s">
         <v>260</v>
@@ -11734,13 +11750,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="19" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B70" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C70" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D70" t="s">
         <v>260</v>
@@ -11748,13 +11764,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="19" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B71" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C71" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="D71" t="s">
         <v>260</v>
@@ -11762,13 +11778,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="19" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="B72" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C72" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="D72" t="s">
         <v>257</v>
@@ -11776,13 +11792,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="19" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B73" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C73" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D73" t="s">
         <v>260</v>
@@ -11790,44 +11806,44 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="19" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B74" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="C74" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D74" t="s">
         <v>260</v>
       </c>
       <c r="E74" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="19" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B75" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C75" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="E75" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="19" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="B76" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="D76" t="s">
         <v>260</v>
@@ -11835,13 +11851,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="19" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B77" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C77" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D77" t="s">
         <v>260</v>
@@ -11849,13 +11865,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="19" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="B78" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C78" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D78" t="s">
         <v>260</v>
@@ -11863,47 +11879,47 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="19" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B79" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C79" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="D79" t="s">
         <v>260</v>
       </c>
       <c r="E79" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="19" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B80" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C80" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D80" t="s">
         <v>260</v>
       </c>
       <c r="E80" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="19" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B81" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="D81" t="s">
         <v>260</v>
@@ -11911,30 +11927,30 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="19" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D82" t="s">
         <v>260</v>
       </c>
       <c r="E82" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="19" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B83" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D83" t="s">
         <v>260</v>
@@ -11942,13 +11958,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="19" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="B84" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="C84" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="D84" t="s">
         <v>260</v>
@@ -11956,13 +11972,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="19" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B85" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C85" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D85" t="s">
         <v>253</v>
@@ -11970,30 +11986,30 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="19" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="B86" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="C86" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D86" t="s">
         <v>258</v>
       </c>
       <c r="E86" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="19" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B87" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C87" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="D87" t="s">
         <v>258</v>
@@ -12001,81 +12017,81 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="19" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="B88" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="C88" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D88" t="s">
         <v>258</v>
       </c>
       <c r="E88" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="19" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B89" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C89" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D89" t="s">
         <v>258</v>
       </c>
       <c r="E89" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="19" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B90" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C90" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="D90" t="s">
         <v>258</v>
       </c>
       <c r="E90" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="19" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="B91" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="C91" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="D91" t="s">
         <v>258</v>
       </c>
       <c r="E91" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="19" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B92" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C92" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D92" t="s">
         <v>258</v>
@@ -12083,13 +12099,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="19" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B93" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="C93" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D93" t="s">
         <v>258</v>
@@ -12097,53 +12113,53 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="19" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="B94" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C94" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D94" t="s">
         <v>258</v>
       </c>
       <c r="E94" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="19" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="B95" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="C95" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="D95" t="s">
         <v>258</v>
       </c>
       <c r="E95" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="19" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="B96" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="C96" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="D96" t="s">
         <v>258</v>
       </c>
       <c r="E96" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>